<commit_message>
v1 - b4 demo
</commit_message>
<xml_diff>
--- a/list_v4.xlsx
+++ b/list_v4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel.araiza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel.araiza\Desktop\denver_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23020B4-3BAB-4121-B657-2F5C6C8B1AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D69018-4B2C-400E-8552-84EB2B5F130F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20595" yWindow="-13365" windowWidth="21600" windowHeight="11175" xr2:uid="{03A9BB32-D70C-4282-83AA-F5181DD7E683}"/>
+    <workbookView xWindow="19845" yWindow="-11715" windowWidth="21600" windowHeight="11175" xr2:uid="{03A9BB32-D70C-4282-83AA-F5181DD7E683}"/>
   </bookViews>
   <sheets>
     <sheet name="list_v4" sheetId="1" r:id="rId1"/>
@@ -2434,7 +2434,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>